<commit_message>
aangepaste PBL na meeting met Bart en Dennis
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Visuals" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$44</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="73">
   <si>
     <t>Feedback</t>
   </si>
@@ -51,21 +51,12 @@
     <t>Alain</t>
   </si>
   <si>
-    <t>Extra gezichten zou voor persoonlijkere touch zorgen</t>
-  </si>
-  <si>
     <t>Katrien</t>
   </si>
   <si>
-    <t>Kegel is een draak</t>
-  </si>
-  <si>
     <t>Resolutie logo niet 100% scherp</t>
   </si>
   <si>
-    <t>Responsiveness</t>
-  </si>
-  <si>
     <t>Kristel</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t>Dennis</t>
   </si>
   <si>
-    <t xml:space="preserve">De hoogte van de 'pagina's' is niet conform een standaard. Normaliter houdt je in een single page website een standaardhoogte aan die je voor iedere 'pagina' gebruikt. Nu heeft iedere 'pagina' een andere hoogte. Dit is zeer vervelend, daar je de muisaanwijzer telkens opnieuw moet positioneren. Een optimale oplossing is het laten aanpassen van de paginahoogte aan de 'viewport' van de gebruiker. Hierdoor wordt de website op ieder platform correct weergegeven en dient er niet naar de navigatieknoppen te worden gescrolld. </t>
-  </si>
-  <si>
     <t xml:space="preserve">De sectie, waar de referenties naar de sociale media in staan, is te smal. Hierdoor worden de cirkels met de icoontjes niet volledig weergegeven. Dit wordt verduidelijkt door de animatie van deze cirkels. </t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t xml:space="preserve">In het nieuwsoverzicht is de CSP-afbeelding van zeer slechte kwaliteit, gebruikt beter de afbeelding die ik aan deze e-mail heb toegevoegd. Hier dient ook bij toekomstige nieuwsitems op gelet te worden. </t>
   </si>
   <si>
-    <t xml:space="preserve">Voor alle drie de vacatures wordt dezelfde afbeelding gebruikt, dit is naar mijn idee niet echt sterk. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tussen de items 'Vacatures' en 'Contact' bestaat een witte lege ruimte. Ik begrijp de achterliggende reden, maar dit ziet er niet echt professioneel uit. Tracht een andere oplossing te bedenken. </t>
   </si>
   <si>
@@ -108,18 +93,12 @@
     <t>Blog Christian.</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>NI</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -144,9 +123,6 @@
     <t>Vacatures vernieuwen</t>
   </si>
   <si>
-    <t>Tim &amp; Joyce</t>
-  </si>
-  <si>
     <t>Referenties - Toelating vragen aan klanten</t>
   </si>
   <si>
@@ -159,9 +135,6 @@
     <t>Wouter</t>
   </si>
   <si>
-    <t>Referenties - template-achtergrond</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -180,18 +153,12 @@
     <t>HIGH</t>
   </si>
   <si>
-    <t>Referenties - template-Design met Elise</t>
-  </si>
-  <si>
     <t>Pijltjes weg</t>
   </si>
   <si>
     <t>Alle titels in het Engels</t>
   </si>
   <si>
-    <t>Google analytics? Cookies??</t>
-  </si>
-  <si>
     <t>"News" verwijderen?</t>
   </si>
   <si>
@@ -219,23 +186,74 @@
     <t>Versie met referenties op tba.bravalco zetten na volgende push to prod</t>
   </si>
   <si>
-    <t>B/D</t>
-  </si>
-  <si>
     <t>Roadmap maken</t>
   </si>
   <si>
-    <t xml:space="preserve">Link met BESPOKE </t>
-  </si>
-  <si>
     <t>Lieve</t>
+  </si>
+  <si>
+    <t>Link met BESPOKE (laatste sectie 'ABOUT')</t>
+  </si>
+  <si>
+    <t>Link naar Sparx</t>
+  </si>
+  <si>
+    <t>Referenties - template-achtergrond (styling light box)</t>
+  </si>
+  <si>
+    <t>Afbeeldingen vacature carousel</t>
+  </si>
+  <si>
+    <t>Kegel vervangen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsiveness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De hoogte van de 'pagina's' is niet conform een standaard. Normaliter houdt je in een single page website een standaardhoogte aan die je voor iedere 'pagina' gebruikt. Nu heeft iedere 'pagina' een andere hoogte. Dit is zeer vervelend, daar je de muisaanwijzer telkens opnieuw moet positioneren. Een optimale oplossing is het laten aanpassen van de paginahoogte aan de 'viewport' van de gebruiker. Hierdoor wordt de website op ieder platform correct weergegeven en dient er niet naar de navigatieknoppen te worden gescrold. </t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>Duplicate (22)</t>
+  </si>
+  <si>
+    <t>Voor alle drie de vacatures wordt dezelfde afbeelding gebruikt, dit is naar mijn idee niet echt sterk. (Aankoop afbeeldingen)</t>
+  </si>
+  <si>
+    <t>Bart / Dennis</t>
+  </si>
+  <si>
+    <t>Duplicate (11)</t>
+  </si>
+  <si>
+    <t>Tim / Nico</t>
+  </si>
+  <si>
+    <t>Tim / Joyce</t>
+  </si>
+  <si>
+    <t>Google analytics &amp; Cookie-wetgeving implementeren</t>
+  </si>
+  <si>
+    <t>De kleuren van het formulier in stijl met website brengen</t>
+  </si>
+  <si>
+    <t>Speciale karakters in formulier accpeteren</t>
+  </si>
+  <si>
+    <t>php foutmelding integreren in foutpagina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,8 +335,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +389,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -396,15 +438,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,18 +539,26 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,14 +580,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>381000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>142879</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>742954</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -956,16 +1023,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="6" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -975,7 +1043,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>0</v>
@@ -993,36 +1061,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1030,15 +1098,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,15 +1114,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="15"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,15 +1132,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,583 +1150,662 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="103.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="147.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="15" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="39.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
         <v>27</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="26" t="s">
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="15" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
         <v>29</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="102" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
-        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="9"/>
+      <c r="D30" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="F30" s="10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>35</v>
+        <v>67</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
+        <v>36</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="22" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="22"/>
+        <v>54</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="D38" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="22"/>
+        <v>55</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="E39" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="28"/>
+        <v>40</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
-        <v>39</v>
-      </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
+        <v>41</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-    </row>
+      <c r="F41" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>42</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:F41"/>
+  <autoFilter ref="A1:F44">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Doing"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1683,13 +1834,13 @@
     </row>
     <row r="17" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B17" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added lost correction of the social icons - Pull menu collapses from now on when an item is clicked - Added 8 new backlog items (mainly linked to the references)
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Visuals" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
   <si>
     <t>Feedback</t>
   </si>
@@ -246,16 +246,40 @@
     <t>php foutmelding integreren in foutpagina</t>
   </si>
   <si>
-    <t>Release</t>
-  </si>
-  <si>
     <t>Voor alle drie de vacatures wordt dezelfde afbeelding gebruikt, dit is naar mijn idee niet echt sterk. (Afbeeldingen vervangen)</t>
+  </si>
+  <si>
+    <t>Bug: JavaScript - 'google' is undefined</t>
+  </si>
+  <si>
+    <t>To release</t>
+  </si>
+  <si>
+    <t>Bug: Het item 'News' heeft geen grijze achtergrond</t>
+  </si>
+  <si>
+    <t>Geen Zwitserse vlag voor het openen van de referenties</t>
+  </si>
+  <si>
+    <t>Lay-out referenties aanpassen overeenkomstig afspraken</t>
+  </si>
+  <si>
+    <t>Bug: Referenties niet correct uitgelijnd (lege plaatsen)</t>
+  </si>
+  <si>
+    <t>Bug: Alle items na 'References' houden de breedte van het betreffende item aan. Ook eindigt de footer voortaan voor het einde van de pagina.</t>
+  </si>
+  <si>
+    <t>Bug: Bij de mobile weergave vallen de 'News' en 'Jobs' pijltjes onder de titel van het volgende item. Bij een versmalde  weergave komen deze te dicht bij elkaar.</t>
+  </si>
+  <si>
+    <t>Bug: Pull-menu wordt te laat weergegeven met nieuwe menu-items</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +424,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -457,7 +486,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -465,6 +494,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -554,11 +584,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
+    <cellStyle name="Accent6" xfId="7" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
@@ -1029,21 +1060,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,7 +1452,7 @@
         <v>40</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1429,7 +1460,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>11</v>
@@ -1578,8 +1609,8 @@
       <c r="E30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>35</v>
+      <c r="F30" s="27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1596,8 +1627,8 @@
       <c r="E31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="27" t="s">
-        <v>28</v>
+      <c r="F31" s="31" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,9 +1642,7 @@
       <c r="D32" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="10" t="s">
         <v>35</v>
       </c>
@@ -1795,15 +1824,127 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
+      <c r="A43" s="13">
+        <v>43</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>44</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>45</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>46</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>47</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>48</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>49</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <v>50</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F44"/>
+  <autoFilter ref="A1:F52"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
google analytics, cookiewet, fotos vacatures
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="PBL II" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$52</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="84">
   <si>
     <t>Feedback</t>
   </si>
@@ -274,12 +269,18 @@
   </si>
   <si>
     <t>Bug: Pull-menu wordt te laat weergegeven met nieuwe menu-items</t>
+  </si>
+  <si>
+    <t>Meer info vereist</t>
+  </si>
+  <si>
+    <t>Krijg het niet opgelost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +430,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -496,7 +503,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,6 +594,7 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Accent6" xfId="7" builtinId="49"/>
@@ -623,8 +631,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>142879</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>733429</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>105899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1052,7 +1060,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1060,11 +1068,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1086,7 @@
     <col min="6" max="6" width="14.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1163,7 +1172,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1193,11 +1202,14 @@
         <v>49</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>8</v>
       </c>
@@ -1215,7 +1227,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>9</v>
       </c>
@@ -1233,7 +1245,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>10</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>11</v>
       </c>
@@ -1273,7 +1285,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>12</v>
       </c>
@@ -1291,7 +1303,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>13</v>
       </c>
@@ -1309,7 +1321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>14</v>
       </c>
@@ -1327,7 +1339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>15</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>16</v>
       </c>
@@ -1361,7 +1373,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -1379,7 +1391,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="103.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="103.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>18</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="147.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="147.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -1435,7 +1447,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>21</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>22</v>
       </c>
@@ -1469,11 +1481,11 @@
         <v>49</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>23</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="39" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="39" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -1509,7 +1521,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>25</v>
       </c>
@@ -1527,7 +1539,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="27" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -1545,7 +1557,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="26.25" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>27</v>
       </c>
@@ -1563,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>28</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>29</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>30</v>
       </c>
@@ -1612,8 +1624,11 @@
       <c r="F30" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>31</v>
       </c>
@@ -1631,7 +1646,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>32</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -1663,7 +1678,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>34</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>35</v>
       </c>
@@ -1693,8 +1708,8 @@
       <c r="E35" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="27" t="s">
-        <v>28</v>
+      <c r="F35" s="31" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1713,7 +1728,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>37</v>
       </c>
@@ -1729,7 +1744,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>38</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>39</v>
       </c>
@@ -1823,7 +1838,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43</v>
       </c>
@@ -1837,7 +1852,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>44</v>
       </c>
@@ -1851,7 +1866,7 @@
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>45</v>
       </c>
@@ -1865,7 +1880,7 @@
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>46</v>
       </c>
@@ -1879,7 +1894,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>47</v>
       </c>
@@ -1893,7 +1908,7 @@
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>48</v>
       </c>
@@ -1907,7 +1922,7 @@
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>49</v>
       </c>
@@ -1921,7 +1936,7 @@
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>50</v>
       </c>
@@ -1935,7 +1950,7 @@
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="18"/>
       <c r="C51" s="19"/>
@@ -1943,8 +1958,16 @@
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
     </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:F52"/>
+  <autoFilter ref="A1:F52">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Bart"/>
+        <filter val="Dennis"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
- Added four new backlog items (of which one has been resolved already) - Rectified the references used by the cookie law implementation - Removed the gray background once an item becomes active
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="PBL II" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Referenties" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$56</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
   <si>
     <t>Feedback</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Meer info vereist</t>
   </si>
   <si>
-    <t>Krijg het niet opgelost</t>
-  </si>
-  <si>
     <t>Sparx (Official partnership)</t>
   </si>
   <si>
@@ -398,12 +395,27 @@
   </si>
   <si>
     <t>Logo</t>
+  </si>
+  <si>
+    <t>Bug: Implementatie cookie-wetgeving functioneert niet door incorrecte referenties. De website wacht met laden tot de referenties een time-out hebben veroorzaakt.</t>
+  </si>
+  <si>
+    <t>Implementatie cookie-wetgeving overeen laten stemmen met lay-out website.</t>
+  </si>
+  <si>
+    <t>Eigen pagina voorzien met toelichting over het gebruik van cookies. (Verplicht)</t>
+  </si>
+  <si>
+    <t>Uitlijning van het item 'Jobs' herzien.</t>
+  </si>
+  <si>
+    <t>Duplicate (6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -944,7 +956,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1057,21 +1069,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,6 +1096,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1612,12 +1625,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1666,7 +1678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1747,7 +1759,7 @@
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>40</v>
@@ -1759,7 +1771,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>8</v>
       </c>
@@ -1777,7 +1789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>9</v>
       </c>
@@ -1835,7 +1847,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>12</v>
       </c>
@@ -1853,7 +1865,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>13</v>
       </c>
@@ -1871,7 +1883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>14</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="90.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>15</v>
       </c>
@@ -1905,7 +1917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="39.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>16</v>
       </c>
@@ -1923,7 +1935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="77.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -1961,7 +1973,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="147.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="147.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -1979,7 +1991,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.25" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>21</v>
       </c>
@@ -2053,7 +2065,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="39" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="39" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>25</v>
       </c>
@@ -2089,7 +2101,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="27" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -2107,7 +2119,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26.25" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>27</v>
       </c>
@@ -2125,7 +2137,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>28</v>
       </c>
@@ -2145,7 +2157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>29</v>
       </c>
@@ -2168,19 +2180,17 @@
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="52"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>31</v>
       </c>
@@ -2198,7 +2208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>32</v>
       </c>
@@ -2214,7 +2224,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -2246,7 +2256,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>35</v>
       </c>
@@ -2264,7 +2274,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>36</v>
       </c>
@@ -2280,7 +2290,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>37</v>
       </c>
@@ -2458,7 +2468,9 @@
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
+      <c r="F47" s="30" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
@@ -2502,25 +2514,76 @@
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>51</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
+        <v>52</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>53</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <v>54</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F52">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="Doing"/>
-        <filter val="On Hold"/>
-        <filter val="To release"/>
-        <filter val="Waiting"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F56"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2530,9 +2593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B14:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2559,12 +2620,12 @@
     </row>
     <row r="36" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B36" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B50" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2578,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,249 +2655,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56" t="s">
-        <v>92</v>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51" t="s">
+        <v>91</v>
       </c>
       <c r="F2" s="38" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="56"/>
+      <c r="B3" s="48" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="53" t="s">
+      <c r="C3" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="56"/>
+      <c r="B4" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="46" t="s">
+      <c r="C4" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="56"/>
+      <c r="B5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="41" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="46"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="53" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="56"/>
+      <c r="B6" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="53" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="56"/>
+      <c r="B7" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="46"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="53" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="56"/>
+      <c r="B8" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="46"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="53" t="s">
+      <c r="C8" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="46" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="56"/>
+      <c r="B9" s="48" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="53" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="56"/>
+      <c r="B10" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="46"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="53" t="s">
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56"/>
+      <c r="B11" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="53" t="s">
+      <c r="C11" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="56"/>
+      <c r="B12" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="46" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57"/>
+      <c r="B13" s="49" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="46"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
-      <c r="B13" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="C14" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="35"/>
       <c r="G14" s="40"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="53" t="s">
+      <c r="A15" s="56"/>
+      <c r="B15" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
+      <c r="B16" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="53" t="s">
+      <c r="C16" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="57"/>
+      <c r="B17" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="54" t="s">
+      <c r="C17" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="47" t="s">
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="48"/>
+      <c r="G17" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
PBL aangepast cfr overleg met Dennis en Bart
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Referenties" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$61</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="131">
   <si>
     <t>Feedback</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Alle titels in het Engels</t>
   </si>
   <si>
-    <t>"News" verwijderen?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Services&amp;Solutions - De representatie van de services en solutions zou ik persoonlijk volledig anders aanpakken. Ten eerste vind ik het vreemd dat het item wordt begonnen met een beeldvullende foto, waar dat voor de andere items niet het geval is. Verder zou ik de services en solutions in het framework aanklikbaar maken, waarmee direct naar het betreffende item kan worden genavigeerd. Nog beter zou zijn, om de beschrijving van de services en solutions in een lightbox te openen, wanneer er in het framework wordt geklikt. Nu moet je de volledige pagina afgaan, in afwachting van de service of solution waar je interesse in hebt. </t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Lieve</t>
   </si>
   <si>
-    <t>Link met BESPOKE (laatste sectie 'ABOUT')</t>
-  </si>
-  <si>
     <t>Link naar Sparx</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>Duplicate (11)</t>
   </si>
   <si>
-    <t>Tim / Nico</t>
-  </si>
-  <si>
     <t>Tim / Joyce</t>
   </si>
   <si>
@@ -277,18 +268,12 @@
     <t>Bug: Pull-menu wordt te laat weergegeven met nieuwe menu-items</t>
   </si>
   <si>
-    <t>Meer info vereist</t>
-  </si>
-  <si>
     <t>Sparx (Official partnership)</t>
   </si>
   <si>
     <t>Certified Scrum Masters &amp; Product Owners</t>
   </si>
   <si>
-    <t>Tim/Elise</t>
-  </si>
-  <si>
     <t>Klant</t>
   </si>
   <si>
@@ -410,12 +395,39 @@
   </si>
   <si>
     <t>Duplicate (6)</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>"News" verwijderen? En vervangen door Partners; Sparx / Bespoke / Cronos / Slingshot</t>
+  </si>
+  <si>
+    <t>Duplicate (34)</t>
+  </si>
+  <si>
+    <t>Link met BESPOKE (laatste sectie 'ABOUT') / tekst en logo optimaliseren zowel in PARTNERS als in BUSINESS ARCHITECTUUR; Aanpassen logo</t>
+  </si>
+  <si>
+    <t>Tekst Business Architecture aanpassen</t>
+  </si>
+  <si>
+    <t>Adres Leuven toevoegen (Adressen onder elkaar en Cronos Leuven niet vermelden)</t>
+  </si>
+  <si>
+    <t>Toevoegen van referenties (vierkant logo van K&amp;G)</t>
+  </si>
+  <si>
+    <t>Foto van product owner qua formaat wat aanpassen zodat dit evengroot is als de 2 anderen</t>
+  </si>
+  <si>
+    <t>Tekst van cookies wit maken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,7 +541,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,12 +595,6 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -1047,7 +1053,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,6 +1117,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1625,17 +1633,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="79.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="11" bestFit="1" customWidth="1"/>
@@ -1705,7 +1713,7 @@
       <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="26" t="s">
@@ -1743,7 +1751,7 @@
       <c r="D6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="26" t="s">
@@ -1755,21 +1763,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>82</v>
-      </c>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
@@ -1794,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>6</v>
@@ -1804,7 +1810,7 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1812,7 +1818,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>7</v>
@@ -1824,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1832,7 +1838,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>7</v>
@@ -1844,7 +1850,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1870,7 +1876,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>9</v>
@@ -1906,7 +1912,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>11</v>
@@ -1914,7 +1920,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="9"/>
       <c r="F15" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -1958,7 +1964,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>11</v>
@@ -1970,7 +1976,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="147.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1996,7 +2002,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>11</v>
@@ -2014,7 +2020,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>11</v>
@@ -2026,7 +2032,7 @@
         <v>40</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2034,17 +2040,17 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2052,7 +2058,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>11</v>
@@ -2062,7 +2068,7 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickTop="1" x14ac:dyDescent="0.25">
@@ -2112,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="17" t="s">
@@ -2145,16 +2151,16 @@
         <v>30</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="27" t="s">
-        <v>28</v>
+      <c r="F28" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2176,7 +2182,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
@@ -2186,9 +2192,9 @@
         <v>40</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="52"/>
+        <v>71</v>
+      </c>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
@@ -2205,7 +2211,7 @@
         <v>40</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2217,7 +2223,7 @@
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="10" t="s">
@@ -2237,23 +2243,23 @@
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2261,17 +2267,17 @@
         <v>35</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,23 +2285,23 @@
         <v>36</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" s="23"/>
-      <c r="F36" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>37</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="22" t="s">
@@ -2306,32 +2312,32 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>38</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22" t="s">
@@ -2340,8 +2346,8 @@
       <c r="E39" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="27" t="s">
-        <v>28</v>
+      <c r="F39" s="30" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2349,7 +2355,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>11</v>
@@ -2369,7 +2375,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22" t="s">
@@ -2387,7 +2393,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22" t="s">
@@ -2405,7 +2411,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>11</v>
@@ -2419,7 +2425,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>11</v>
@@ -2433,7 +2439,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>11</v>
@@ -2447,7 +2453,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>11</v>
@@ -2461,7 +2467,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>11</v>
@@ -2469,7 +2475,7 @@
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
       <c r="F47" s="30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2477,7 +2483,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>11</v>
@@ -2491,7 +2497,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>11</v>
@@ -2505,7 +2511,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>11</v>
@@ -2519,7 +2525,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>11</v>
@@ -2529,7 +2535,7 @@
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2537,7 +2543,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>11</v>
@@ -2551,7 +2557,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>11</v>
@@ -2565,25 +2571,121 @@
         <v>54</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
+      <c r="D54" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
+      <c r="A55" s="13">
+        <v>55</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
+        <v>56</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
+        <v>57</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
+        <v>58</v>
+      </c>
+      <c r="B58" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
+        <v>59</v>
+      </c>
+      <c r="B59" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F56"/>
+  <autoFilter ref="A1:F61"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2593,7 +2695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B14:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2619,13 +2723,13 @@
       </c>
     </row>
     <row r="36" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B36" s="34" t="s">
-        <v>83</v>
+      <c r="B36" s="33" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B50" s="34" t="s">
-        <v>84</v>
+      <c r="B50" s="33" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2655,249 +2759,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="36" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" s="36" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="55"/>
+      <c r="B3" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="C3" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="55"/>
+      <c r="B4" s="47" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="C4" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="55"/>
+      <c r="B5" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="55"/>
+      <c r="B6" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="55"/>
+      <c r="B7" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="55"/>
+      <c r="B8" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="55"/>
+      <c r="B9" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="55"/>
+      <c r="B10" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="55"/>
+      <c r="B11" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="55"/>
+      <c r="B12" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="56"/>
+      <c r="B13" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="55"/>
+      <c r="B15" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="55"/>
+      <c r="B16" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="41"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="41"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="41"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="41"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="41"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="C16" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="G16" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="56"/>
+      <c r="B17" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C17" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="40"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="41"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="43"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added new lightbox based on existing bootstrap scripts.
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="PBL II" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1137,9 +1137,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,12 +1154,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1669,9 +1669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,8 +1806,8 @@
       <c r="E7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>28</v>
+      <c r="F7" s="31" t="s">
+        <v>71</v>
       </c>
       <c r="G7" s="51"/>
     </row>
@@ -2777,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,10 +2793,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="53" t="s">
         <v>82</v>
       </c>
@@ -2814,7 +2814,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="46" t="s">
@@ -2837,7 +2837,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="47" t="s">
         <v>88</v>
       </c>
@@ -2857,7 +2857,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="47" t="s">
         <v>89</v>
       </c>
@@ -2870,7 +2870,7 @@
       <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="47" t="s">
         <v>90</v>
       </c>
@@ -2887,12 +2887,12 @@
       <c r="G5" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="54" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="47" t="s">
         <v>91</v>
       </c>
@@ -2903,7 +2903,7 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="47" t="s">
         <v>92</v>
       </c>
@@ -2914,7 +2914,7 @@
       <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="47" t="s">
         <v>93</v>
       </c>
@@ -2929,12 +2929,12 @@
       <c r="G8" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="54" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="47" t="s">
         <v>97</v>
       </c>
@@ -2945,7 +2945,7 @@
       <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="47" t="s">
         <v>98</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="47" t="s">
         <v>99</v>
       </c>
@@ -2975,7 +2975,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="47" t="s">
         <v>100</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="48" t="s">
         <v>103</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="57" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="49" t="s">
@@ -3012,7 +3012,7 @@
       <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="47" t="s">
         <v>108</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="G15" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="47" t="s">
         <v>109</v>
       </c>
@@ -3044,7 +3044,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="48" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
aanpassingen zie backlog to release en mail 20170926
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -17,7 +12,7 @@
     <sheet name="Referenties" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$63</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="138">
   <si>
     <t>Feedback</t>
   </si>
@@ -437,12 +432,18 @@
   </si>
   <si>
     <t>Olivier</t>
+  </si>
+  <si>
+    <t>bug jobs, contact en footer sectie breder gemaakt (cfr services en solutions</t>
+  </si>
+  <si>
+    <t>zwitserse vlag weg bij referentie K&amp;G als voorbeeld + ander hoover effect (shrink)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1659,7 +1660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1667,11 +1668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,7 +1976,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>34</v>
       </c>
@@ -2326,8 +2327,8 @@
         <v>48</v>
       </c>
       <c r="E36" s="23"/>
-      <c r="F36" s="27" t="s">
-        <v>28</v>
+      <c r="F36" s="31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2611,13 +2612,13 @@
         <v>11</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F54" s="27" t="s">
-        <v>28</v>
+      <c r="F54" s="31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2634,8 +2635,8 @@
       <c r="E55" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="27" t="s">
-        <v>28</v>
+      <c r="F55" s="31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2652,8 +2653,8 @@
       <c r="E56" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="27" t="s">
-        <v>28</v>
+      <c r="F56" s="31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,8 +2671,8 @@
       <c r="E57" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="27" t="s">
-        <v>28</v>
+      <c r="F57" s="31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2711,15 +2712,51 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="A60" s="13">
+        <v>60</v>
+      </c>
+      <c r="B60" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="13">
+        <v>61</v>
+      </c>
+      <c r="B61" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F61"/>
+  <autoFilter ref="A1:F63"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
lijn 62 toegevoegd, postcode en plaats aanpassen naar '3000 Leuven'
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="Referenties" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$64</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="140">
   <si>
     <t>Feedback</t>
   </si>
@@ -438,6 +443,12 @@
   </si>
   <si>
     <t>zwitserse vlag weg bij referentie K&amp;G als voorbeeld + ander hoover effect (shrink)</t>
+  </si>
+  <si>
+    <t>Adres Cronos Leuven veranderen van '3001 Heverlee' naar '3000 Leuven'</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -557,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +622,11 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -981,7 +997,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -990,8 +1006,9 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1156,8 +1173,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="Accent4" xfId="8" builtinId="41"/>
     <cellStyle name="Accent6" xfId="7" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1660,7 +1681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1668,11 +1689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:F61"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,15 +2769,33 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="A62" s="13">
+        <v>62</v>
+      </c>
+      <c r="B62" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="60" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F63"/>
+  <autoFilter ref="A1:F64"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
3 partners, 2 nieuwe referenties, aantal kleine wijzigingen
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="150">
   <si>
     <t>Feedback</t>
   </si>
@@ -449,13 +444,43 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>Denk dat dit al is opgelost met ander item (jobs sectie en footer is nu volledige breedte van het scherm)</t>
+  </si>
+  <si>
+    <t>enkel tekst moet nog wit gemaakt worden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate (59) </t>
+  </si>
+  <si>
+    <t>To release (54)</t>
+  </si>
+  <si>
+    <t>Duplicate (61)</t>
+  </si>
+  <si>
+    <t>Hoeft niet, is afwisselend grijs/wit, maar gezien de referenties er even tussen uit gehaald zijn klopt dit niet meer, van zodra die er terug in staan is het ok --&gt; niets voor dit item te doen lijkt me</t>
+  </si>
+  <si>
+    <t>3 Referenties (AIV, SFPD, K&amp;G) toevoegen conform lightbox dennis</t>
+  </si>
+  <si>
+    <t>We gingen de about sectie niet aanpassen, maar een sectie partners maken om bespoke in te vermelden (zie item 34)!</t>
+  </si>
+  <si>
+    <t>Ignore (34)</t>
+  </si>
+  <si>
+    <t>Teksten referenties nalezen (PDOS is SFPD geworden, AGIV is AIV geworden) + teksten partners optimaliseren + Deftig LOGO bespoke aanleveren voor partners sectie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,8 +592,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,13 +653,8 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -996,8 +1022,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1006,7 +1041,6 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1057,15 +1091,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1173,12 +1198,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Accent4" xfId="8" builtinId="41"/>
+  <cellStyles count="8">
     <cellStyle name="Accent6" xfId="7" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1681,7 +1714,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1689,11 +1722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,10 +1740,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -1769,10 +1802,10 @@
       <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1790,7 +1823,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1807,10 +1840,10 @@
       <c r="D6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1825,13 +1858,13 @@
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="51"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
@@ -1865,7 +1898,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="27" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1885,7 +1918,7 @@
       <c r="E10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1905,7 +1938,7 @@
       <c r="E11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1975,7 +2008,7 @@
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="25" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2031,7 +2064,7 @@
       <c r="E18" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2087,7 +2120,7 @@
       <c r="E21" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2105,7 +2138,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2123,7 +2156,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2247,10 +2280,10 @@
       <c r="E30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="51"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
@@ -2266,7 +2299,7 @@
       <c r="E31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2286,7 +2319,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -2298,11 +2331,11 @@
         <v>21</v>
       </c>
       <c r="E33" s="9"/>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>34</v>
       </c>
@@ -2313,12 +2346,14 @@
       <c r="D34" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>35</v>
       </c>
@@ -2332,467 +2367,523 @@
       <c r="E35" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>36</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22" t="s">
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="31" t="s">
+      <c r="E36" s="20"/>
+      <c r="F36" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>37</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22" t="s">
+      <c r="C37" s="19"/>
+      <c r="D37" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>38</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="22" t="s">
-        <v>11</v>
+      <c r="D38" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>39</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="27" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>40</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="22" t="s">
+      <c r="C40" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F40" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>41</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="27" t="s">
+      <c r="F41" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>42</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="27" t="s">
+      <c r="F42" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>44</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>45</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="19"/>
+      <c r="F45" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>46</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" s="19"/>
+      <c r="F46" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>47</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="30" t="s">
+      <c r="C47" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>48</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C48" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>49</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-    </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C49" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" s="19"/>
+      <c r="F49" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G49" s="58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>50</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-    </row>
-    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C50" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>51</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="31" t="s">
+      <c r="C51" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="19"/>
+      <c r="F51" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>52</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G52" s="57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>53</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C53" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>54</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="22" t="s">
+      <c r="C54" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>55</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>56</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>57</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22" t="s">
+      <c r="C57" s="19"/>
+      <c r="D57" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>58</v>
       </c>
-      <c r="B58" s="52" t="s">
+      <c r="B58" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22" t="s">
+      <c r="C58" s="19"/>
+      <c r="D58" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="27" t="s">
+      <c r="F58" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>59</v>
       </c>
-      <c r="B59" s="52" t="s">
+      <c r="B59" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22" t="s">
+      <c r="C59" s="19"/>
+      <c r="D59" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F59" s="27" t="s">
+      <c r="F59" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>60</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22" t="s">
+      <c r="C60" s="19"/>
+      <c r="D60" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="31" t="s">
+      <c r="F60" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>61</v>
       </c>
-      <c r="B61" s="52" t="s">
+      <c r="B61" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22" t="s">
+      <c r="C61" s="19"/>
+      <c r="D61" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="F61" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>62</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="B62" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D62" s="22"/>
+      <c r="D62" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="E62" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="60" t="s">
+      <c r="F62" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
+        <v>63</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="13">
+        <v>64</v>
+      </c>
+      <c r="B64" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F64"/>
@@ -2833,12 +2924,12 @@
       </c>
     </row>
     <row r="36" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="30" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2869,63 +2960,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="53" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="35" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41" t="s">
         <v>86</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="37" t="s">
         <v>113</v>
       </c>
       <c r="H3" t="s">
@@ -2933,206 +3024,206 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="47" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="40"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="47" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="41" t="s">
         <v>86</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="51" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="55"/>
+      <c r="B6" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="40"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="47" t="s">
+      <c r="A7" s="55"/>
+      <c r="B7" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="40"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="47" t="s">
+      <c r="A8" s="55"/>
+      <c r="B8" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="51" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="47" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="40"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="47" t="s">
+      <c r="A10" s="55"/>
+      <c r="B10" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="37" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="47" t="s">
+      <c r="A11" s="55"/>
+      <c r="B11" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="37" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="47" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="40"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="56"/>
+      <c r="B13" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="47" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="40"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="47" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="41" t="s">
         <v>86</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="48" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="41" t="s">
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
aanpassingen ikv vacature lightbox en job carroussel
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="150">
   <si>
     <t>Feedback</t>
   </si>
@@ -1183,6 +1183,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1197,18 +1209,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1714,7 +1714,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1725,8 +1725,8 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>22</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>23</v>
       </c>
@@ -2153,14 +2153,16 @@
         <v>11</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="39" thickTop="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -2614,7 +2616,7 @@
       <c r="F49" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="G49" s="58" t="s">
+      <c r="G49" s="53" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2665,7 +2667,7 @@
       <c r="F52" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="G52" s="57" t="s">
+      <c r="G52" s="52" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2766,13 +2768,13 @@
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="24" t="s">
-        <v>28</v>
+      <c r="F58" s="28" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2871,7 +2873,7 @@
       <c r="A64" s="13">
         <v>64</v>
       </c>
-      <c r="B64" s="60" t="s">
+      <c r="B64" s="55" t="s">
         <v>149</v>
       </c>
       <c r="C64" s="19"/>
@@ -2881,7 +2883,7 @@
       <c r="E64" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="59" t="s">
+      <c r="F64" s="54" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2960,10 +2962,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="50" t="s">
         <v>82</v>
       </c>
@@ -2981,7 +2983,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="58" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3004,7 +3006,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="44" t="s">
         <v>88</v>
       </c>
@@ -3024,7 +3026,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="44" t="s">
         <v>89</v>
       </c>
@@ -3037,7 +3039,7 @@
       <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="44" t="s">
         <v>90</v>
       </c>
@@ -3059,7 +3061,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="44" t="s">
         <v>91</v>
       </c>
@@ -3070,7 +3072,7 @@
       <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="44" t="s">
         <v>92</v>
       </c>
@@ -3081,7 +3083,7 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="44" t="s">
         <v>93</v>
       </c>
@@ -3101,7 +3103,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="44" t="s">
         <v>97</v>
       </c>
@@ -3112,7 +3114,7 @@
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="44" t="s">
         <v>98</v>
       </c>
@@ -3125,7 +3127,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="44" t="s">
         <v>99</v>
       </c>
@@ -3142,7 +3144,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="44" t="s">
         <v>100</v>
       </c>
@@ -3153,7 +3155,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="56"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="45" t="s">
         <v>103</v>
       </c>
@@ -3164,7 +3166,7 @@
       <c r="G13" s="39"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="58" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -3179,7 +3181,7 @@
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="44" t="s">
         <v>108</v>
       </c>
@@ -3190,7 +3192,7 @@
       <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="44" t="s">
         <v>109</v>
       </c>
@@ -3211,7 +3213,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="45" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
excel backlog nog wat aangepast
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
   <si>
     <t>Feedback</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t>Teksten referenties nalezen (PDOS is SFPD geworden, AGIV is AIV geworden) + teksten partners optimaliseren + Deftig LOGO bespoke aanleveren voor partners sectie</t>
+  </si>
+  <si>
+    <t>BA en Product owner conform FA implementeren (lightbox) van zodra FA goedgekeurd is</t>
+  </si>
+  <si>
+    <t>Nog even on hold totdat item 23 goedgekeurd is!</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1031,6 +1037,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1042,7 +1074,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1189,12 +1221,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1208,6 +1234,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1714,7 +1752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1722,11 +1760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,18 +2911,94 @@
       <c r="A64" s="13">
         <v>64</v>
       </c>
-      <c r="B64" s="55" t="s">
+      <c r="B64" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19" t="s">
+      <c r="C64" s="60"/>
+      <c r="D64" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="54" t="s">
+      <c r="F64" s="62" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="13">
+        <v>65</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E65" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="13">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="13">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="13">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="13">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2962,10 +3076,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="50" t="s">
         <v>82</v>
       </c>
@@ -2983,7 +3097,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="56" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3006,7 +3120,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="44" t="s">
         <v>88</v>
       </c>
@@ -3026,7 +3140,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="44" t="s">
         <v>89</v>
       </c>
@@ -3039,7 +3153,7 @@
       <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="44" t="s">
         <v>90</v>
       </c>
@@ -3061,7 +3175,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="44" t="s">
         <v>91</v>
       </c>
@@ -3072,7 +3186,7 @@
       <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="44" t="s">
         <v>92</v>
       </c>
@@ -3083,7 +3197,7 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="44" t="s">
         <v>93</v>
       </c>
@@ -3103,7 +3217,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="44" t="s">
         <v>97</v>
       </c>
@@ -3114,7 +3228,7 @@
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="44" t="s">
         <v>98</v>
       </c>
@@ -3127,7 +3241,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="44" t="s">
         <v>99</v>
       </c>
@@ -3144,7 +3258,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="44" t="s">
         <v>100</v>
       </c>
@@ -3155,7 +3269,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="45" t="s">
         <v>103</v>
       </c>
@@ -3166,7 +3280,7 @@
       <c r="G13" s="39"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="56" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -3181,7 +3295,7 @@
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="44" t="s">
         <v>108</v>
       </c>
@@ -3192,7 +3306,7 @@
       <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="44" t="s">
         <v>109</v>
       </c>
@@ -3213,7 +3327,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="45" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
po en ba vacature ook in lightbox
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Referenties" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PBL II'!$A$1:$F$76</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="153">
   <si>
     <t>Feedback</t>
   </si>
@@ -479,7 +479,10 @@
     <t>BA en Product owner conform FA implementeren (lightbox) van zodra FA goedgekeurd is</t>
   </si>
   <si>
-    <t>Nog even on hold totdat item 23 goedgekeurd is!</t>
+    <t>PDF voorzien voor vacature product owner conform fa en ba (hetgeen achter de afprinten knop van de lightbox zit)</t>
+  </si>
+  <si>
+    <t>Wat wordt hiermee bedoelt?</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1077,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1221,6 +1224,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,18 +1255,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1763,8 +1772,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2475,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>39</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>40</v>
       </c>
@@ -2500,11 +2509,14 @@
       <c r="E40" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>41</v>
       </c>
@@ -2911,98 +2923,108 @@
       <c r="A64" s="13">
         <v>64</v>
       </c>
-      <c r="B64" s="59" t="s">
+      <c r="B64" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60" t="s">
+      <c r="C64" s="55"/>
+      <c r="D64" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E64" s="61" t="s">
+      <c r="E64" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="62" t="s">
+      <c r="F64" s="57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>65</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15" t="s">
+      <c r="C65" s="59"/>
+      <c r="D65" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E65" s="61" t="s">
+      <c r="E65" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F65" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F65" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F64"/>
+  <autoFilter ref="A1:F76"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3076,10 +3098,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="50" t="s">
         <v>82</v>
       </c>
@@ -3097,7 +3119,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="62" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3120,7 +3142,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="44" t="s">
         <v>88</v>
       </c>
@@ -3140,7 +3162,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="44" t="s">
         <v>89</v>
       </c>
@@ -3153,7 +3175,7 @@
       <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="44" t="s">
         <v>90</v>
       </c>
@@ -3175,7 +3197,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="44" t="s">
         <v>91</v>
       </c>
@@ -3186,7 +3208,7 @@
       <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="44" t="s">
         <v>92</v>
       </c>
@@ -3197,7 +3219,7 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="44" t="s">
         <v>93</v>
       </c>
@@ -3217,7 +3239,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="44" t="s">
         <v>97</v>
       </c>
@@ -3228,7 +3250,7 @@
       <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="44" t="s">
         <v>98</v>
       </c>
@@ -3241,7 +3263,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="44" t="s">
         <v>99</v>
       </c>
@@ -3258,7 +3280,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="44" t="s">
         <v>100</v>
       </c>
@@ -3269,7 +3291,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="45" t="s">
         <v>103</v>
       </c>
@@ -3280,7 +3302,7 @@
       <c r="G13" s="39"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -3295,7 +3317,7 @@
       <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="44" t="s">
         <v>108</v>
       </c>
@@ -3306,7 +3328,7 @@
       <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="44" t="s">
         <v>109</v>
       </c>
@@ -3327,7 +3349,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="45" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
filter voor referenties tijdelijk in commentaar gezet
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="155">
   <si>
     <t>Feedback</t>
   </si>
@@ -483,6 +483,12 @@
   </si>
   <si>
     <t>Wat wordt hiermee bedoelt?</t>
+  </si>
+  <si>
+    <t>Filter voor referenties ALL/PUBLIC/PRIVATE terug enablen indien meer referenties aanwezig (momenteel code in commentaar gezet)</t>
+  </si>
+  <si>
+    <t>NEw</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1772,8 +1778,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,11 +2965,11 @@
       <c r="A66" s="13">
         <v>66</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15" t="s">
+      <c r="C66" s="59"/>
+      <c r="D66" s="59" t="s">
         <v>21</v>
       </c>
       <c r="E66" s="56" t="s">
@@ -2973,55 +2979,111 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>67</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>68</v>
       </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>69</v>
       </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>70</v>
       </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>71</v>
       </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>72</v>
       </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>73</v>
       </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>74</v>
       </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>75</v>
       </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
         <v>76</v>
       </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F76"/>

</xml_diff>

<commit_message>
backlog up to date gezet na prd release
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="152">
   <si>
     <t>Feedback</t>
   </si>
@@ -209,15 +209,9 @@
     <t>Waiting</t>
   </si>
   <si>
-    <t>Duplicate (22)</t>
-  </si>
-  <si>
     <t>Bart / Dennis</t>
   </si>
   <si>
-    <t>Duplicate (11)</t>
-  </si>
-  <si>
     <t>Tim / Joyce</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>Bug: JavaScript - 'google' is undefined</t>
   </si>
   <si>
-    <t>To release</t>
-  </si>
-  <si>
     <t>Bug: Het item 'News' heeft geen grijze achtergrond</t>
   </si>
   <si>
@@ -386,18 +377,12 @@
     <t>Eigen pagina voorzien met toelichting over het gebruik van cookies. (Verplicht)</t>
   </si>
   <si>
-    <t>Duplicate (6)</t>
-  </si>
-  <si>
     <t>Kevin</t>
   </si>
   <si>
     <t>"News" verwijderen? En vervangen door Partners; Sparx / Bespoke / Cronos / Slingshot</t>
   </si>
   <si>
-    <t>Duplicate (34)</t>
-  </si>
-  <si>
     <t>Link met BESPOKE (laatste sectie 'ABOUT') / tekst en logo optimaliseren zowel in PARTNERS als in BUSINESS ARCHITECTUUR; Aanpassen logo</t>
   </si>
   <si>
@@ -446,21 +431,6 @@
     <t>New</t>
   </si>
   <si>
-    <t>Denk dat dit al is opgelost met ander item (jobs sectie en footer is nu volledige breedte van het scherm)</t>
-  </si>
-  <si>
-    <t>enkel tekst moet nog wit gemaakt worden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicate (59) </t>
-  </si>
-  <si>
-    <t>To release (54)</t>
-  </si>
-  <si>
-    <t>Duplicate (61)</t>
-  </si>
-  <si>
     <t>Hoeft niet, is afwisselend grijs/wit, maar gezien de referenties er even tussen uit gehaald zijn klopt dit niet meer, van zodra die er terug in staan is het ok --&gt; niets voor dit item te doen lijkt me</t>
   </si>
   <si>
@@ -470,9 +440,6 @@
     <t>We gingen de about sectie niet aanpassen, maar een sectie partners maken om bespoke in te vermelden (zie item 34)!</t>
   </si>
   <si>
-    <t>Ignore (34)</t>
-  </si>
-  <si>
     <t>Teksten referenties nalezen (PDOS is SFPD geworden, AGIV is AIV geworden) + teksten partners optimaliseren + Deftig LOGO bespoke aanleveren voor partners sectie</t>
   </si>
   <si>
@@ -482,13 +449,37 @@
     <t>PDF voorzien voor vacature product owner conform fa en ba (hetgeen achter de afprinten knop van de lightbox zit)</t>
   </si>
   <si>
-    <t>Wat wordt hiermee bedoelt?</t>
-  </si>
-  <si>
     <t>Filter voor referenties ALL/PUBLIC/PRIVATE terug enablen indien meer referenties aanwezig (momenteel code in commentaar gezet)</t>
   </si>
   <si>
-    <t>NEw</t>
+    <t>release 15/11</t>
+  </si>
+  <si>
+    <t>Denk dat dit al is opgelost met ander item (jobs sectie en footer is nu volledige breedte van het scherm) --&gt; item 54 (release 15/11)</t>
+  </si>
+  <si>
+    <t>duplicate 22</t>
+  </si>
+  <si>
+    <t>Duplicate 11</t>
+  </si>
+  <si>
+    <t>Duplicate 34</t>
+  </si>
+  <si>
+    <t>Duplicate 61</t>
+  </si>
+  <si>
+    <t>Duplicate 6</t>
+  </si>
+  <si>
+    <t>enkel tekst moet nog wit gemaakt worden (duplicate 59)</t>
+  </si>
+  <si>
+    <t>Duplicate 33</t>
+  </si>
+  <si>
+    <t>Wat wordt hiermee bedoeld?</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1074,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1157,12 +1148,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
@@ -1214,7 +1199,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1223,9 +1207,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1767,7 +1748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1775,11 +1756,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1828,7 +1810,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1855,7 +1837,7 @@
       <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="23" t="s">
@@ -1880,7 +1862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1893,14 +1875,14 @@
       <c r="D6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1911,15 +1893,17 @@
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="48"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>8</v>
       </c>
@@ -1937,7 +1921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>9</v>
       </c>
@@ -1951,8 +1935,11 @@
         <v>21</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="27" t="s">
-        <v>61</v>
+      <c r="F9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1975,7 +1962,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>11</v>
       </c>
@@ -1991,11 +1978,14 @@
       <c r="E11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>12</v>
       </c>
@@ -2013,7 +2003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>13</v>
       </c>
@@ -2027,11 +2017,11 @@
         <v>23</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>14</v>
       </c>
@@ -2049,7 +2039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="78" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>15</v>
       </c>
@@ -2065,7 +2055,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="39.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>16</v>
       </c>
@@ -2083,7 +2073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="64.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -2121,7 +2111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="147.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="147.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -2139,7 +2129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="27" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -2157,7 +2147,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="27.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>21</v>
       </c>
@@ -2173,16 +2163,19 @@
       <c r="E21" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="27" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>11</v>
@@ -2191,11 +2184,14 @@
         <v>48</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>23</v>
       </c>
@@ -2211,11 +2207,14 @@
       <c r="E23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>25</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -2262,14 +2261,14 @@
         <v>11</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>27</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>28</v>
       </c>
@@ -2295,10 +2294,10 @@
         <v>30</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>40</v>
@@ -2307,7 +2306,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>29</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>30</v>
       </c>
@@ -2335,12 +2334,14 @@
       <c r="E30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="48"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>31</v>
       </c>
@@ -2354,11 +2355,14 @@
       <c r="E31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>32</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -2386,16 +2390,19 @@
         <v>21</v>
       </c>
       <c r="E33" s="9"/>
-      <c r="F33" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
@@ -2404,29 +2411,35 @@
       <c r="E34" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>35</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>36</v>
       </c>
@@ -2438,11 +2451,14 @@
         <v>48</v>
       </c>
       <c r="E36" s="20"/>
-      <c r="F36" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>37</v>
       </c>
@@ -2458,15 +2474,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="27.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>38</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>48</v>
@@ -2474,14 +2490,14 @@
       <c r="E38" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>148</v>
+      <c r="F38" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="G38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>39</v>
       </c>
@@ -2495,8 +2511,11 @@
       <c r="E39" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="27" t="s">
-        <v>123</v>
+      <c r="F39" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2504,7 +2523,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>11</v>
@@ -2519,7 +2538,7 @@
         <v>60</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2527,7 +2546,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19" t="s">
@@ -2545,7 +2564,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19" t="s">
@@ -2558,12 +2577,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>43</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>11</v>
@@ -2572,26 +2591,31 @@
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>44</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>45</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>11</v>
@@ -2604,15 +2628,15 @@
         <v>59</v>
       </c>
       <c r="G45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>46</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>11</v>
@@ -2621,24 +2645,30 @@
         <v>48</v>
       </c>
       <c r="E46" s="19"/>
-      <c r="F46" s="27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>47</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="19"/>
-      <c r="F47" s="27" t="s">
-        <v>120</v>
+      <c r="F47" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" s="49" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2646,7 +2676,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>11</v>
@@ -2655,12 +2685,12 @@
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
     </row>
-    <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>49</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>11</v>
@@ -2669,11 +2699,11 @@
         <v>48</v>
       </c>
       <c r="E49" s="19"/>
-      <c r="F49" s="28" t="s">
+      <c r="F49" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49" s="49" t="s">
         <v>143</v>
-      </c>
-      <c r="G49" s="53" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -2681,7 +2711,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>11</v>
@@ -2690,12 +2720,12 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
     </row>
-    <row r="51" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>51</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>11</v>
@@ -2704,27 +2734,30 @@
         <v>11</v>
       </c>
       <c r="E51" s="19"/>
-      <c r="F51" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F51" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>52</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="G52" s="52" t="s">
-        <v>141</v>
+      <c r="F52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="49" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2732,7 +2765,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>11</v>
@@ -2741,12 +2774,12 @@
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>54</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>11</v>
@@ -2757,16 +2790,19 @@
       <c r="E54" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F54" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F54" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>55</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19" t="s">
@@ -2775,16 +2811,19 @@
       <c r="E55" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F55" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>56</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19" t="s">
@@ -2793,16 +2832,19 @@
       <c r="E56" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>57</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19" t="s">
@@ -2811,16 +2853,19 @@
       <c r="E57" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>58</v>
       </c>
-      <c r="B58" s="49" t="s">
-        <v>128</v>
+      <c r="B58" s="46" t="s">
+        <v>123</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19" t="s">
@@ -2829,16 +2874,19 @@
       <c r="E58" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="28" t="s">
-        <v>71</v>
+      <c r="F58" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G58" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>59</v>
       </c>
-      <c r="B59" s="49" t="s">
-        <v>129</v>
+      <c r="B59" s="46" t="s">
+        <v>124</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19" t="s">
@@ -2851,12 +2899,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>60</v>
       </c>
-      <c r="B60" s="49" t="s">
-        <v>136</v>
+      <c r="B60" s="46" t="s">
+        <v>131</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="19" t="s">
@@ -2865,16 +2913,19 @@
       <c r="E60" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>61</v>
       </c>
-      <c r="B61" s="49" t="s">
-        <v>137</v>
+      <c r="B61" s="46" t="s">
+        <v>132</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19" t="s">
@@ -2883,16 +2934,19 @@
       <c r="E61" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F61" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G61" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>62</v>
       </c>
-      <c r="B62" s="49" t="s">
-        <v>138</v>
+      <c r="B62" s="46" t="s">
+        <v>133</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>21</v>
@@ -2903,16 +2957,19 @@
       <c r="E62" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F62" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>63</v>
       </c>
-      <c r="B63" s="49" t="s">
-        <v>146</v>
+      <c r="B63" s="46" t="s">
+        <v>136</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19" t="s">
@@ -2921,70 +2978,76 @@
       <c r="E63" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F63" s="28" t="s">
-        <v>71</v>
+      <c r="F63" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>64</v>
       </c>
-      <c r="B64" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="C64" s="55"/>
-      <c r="D64" s="55" t="s">
+      <c r="B64" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E64" s="56" t="s">
+      <c r="E64" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="57" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>65</v>
       </c>
-      <c r="B65" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59" t="s">
+      <c r="B65" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="55"/>
+      <c r="D65" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="E65" s="56" t="s">
+      <c r="E65" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F65" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F65" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
         <v>66</v>
       </c>
-      <c r="B66" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C66" s="59"/>
-      <c r="D66" s="59" t="s">
+      <c r="B66" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E66" s="56" t="s">
+      <c r="E66" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="57" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F66" s="53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>67</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
@@ -2992,10 +3055,10 @@
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>68</v>
       </c>
@@ -3005,7 +3068,7 @@
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>69</v>
       </c>
@@ -3015,7 +3078,7 @@
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>70</v>
       </c>
@@ -3025,7 +3088,7 @@
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>71</v>
       </c>
@@ -3035,7 +3098,7 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>72</v>
       </c>
@@ -3045,7 +3108,7 @@
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>73</v>
       </c>
@@ -3055,7 +3118,7 @@
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>74</v>
       </c>
@@ -3065,7 +3128,7 @@
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>75</v>
       </c>
@@ -3075,7 +3138,7 @@
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
         <v>76</v>
       </c>
@@ -3086,7 +3149,16 @@
       <c r="F76" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F76"/>
+  <autoFilter ref="A1:F76">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="Doing"/>
+        <filter val="New"/>
+        <filter val="On Hold"/>
+        <filter val="Waiting"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3124,13 +3196,13 @@
       </c>
     </row>
     <row r="36" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B36" s="30" t="s">
-        <v>79</v>
+      <c r="B36" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B50" s="30" t="s">
-        <v>80</v>
+      <c r="B50" s="28" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3160,270 +3232,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="50" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="32" t="s">
+      <c r="C2" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="D2" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
+      <c r="B4" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="59"/>
+      <c r="B5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="59"/>
+      <c r="B6" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
+      <c r="B7" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
+      <c r="B8" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
+      <c r="B9" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
+      <c r="B10" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="60"/>
+      <c r="B13" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
-      <c r="B5" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="51" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
-      <c r="B8" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="H8" s="51" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
-      <c r="B9" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="37" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="37"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
-      <c r="B13" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
+      <c r="B15" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="35"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C16" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="44" t="s">
+      <c r="G16" s="35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="60"/>
+      <c r="B17" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
-      <c r="B16" s="44" t="s">
+      <c r="C17" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="38" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="39"/>
+      <c r="G17" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added vector logo of TBA to documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="154">
   <si>
     <t>Feedback</t>
   </si>
@@ -483,12 +488,15 @@
   </si>
   <si>
     <t>User story's aanpassen naar user stories (op 2 plaatsen in jobs sectie)</t>
+  </si>
+  <si>
+    <t>Updaten lay-out referenties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1751,7 +1759,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1762,9 +1770,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,11 +3089,17 @@
       <c r="A69" s="13">
         <v>69</v>
       </c>
-      <c r="B69" s="5"/>
+      <c r="B69" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
+      <c r="D69" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
+      <c r="F69" s="9" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13">

</xml_diff>

<commit_message>
user story's aangepast naar user stories
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aartsde\Documents\Website\trunk\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -496,7 +491,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1759,7 +1754,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1771,8 +1766,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1893,7 +1888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1914,7 +1909,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>8</v>
       </c>
@@ -1932,7 +1927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>9</v>
       </c>
@@ -1973,7 +1968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>11</v>
       </c>
@@ -1996,7 +1991,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>12</v>
       </c>
@@ -2014,7 +2009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>13</v>
       </c>
@@ -2032,7 +2027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>14</v>
       </c>
@@ -2050,7 +2045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="78" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>15</v>
       </c>
@@ -2066,7 +2061,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="39.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>16</v>
       </c>
@@ -2084,7 +2079,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="64.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="147.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="147.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -2140,7 +2135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="27" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -2158,7 +2153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>21</v>
       </c>
@@ -2181,7 +2176,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="27" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>22</v>
       </c>
@@ -2202,7 +2197,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="39.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>23</v>
       </c>
@@ -2225,7 +2220,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="39.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -2243,7 +2238,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>25</v>
       </c>
@@ -2261,7 +2256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>27</v>
       </c>
@@ -2297,7 +2292,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>28</v>
       </c>
@@ -2317,7 +2312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>29</v>
       </c>
@@ -2331,7 +2326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>30</v>
       </c>
@@ -2352,7 +2347,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>31</v>
       </c>
@@ -2373,7 +2368,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>32</v>
       </c>
@@ -2389,7 +2384,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -2408,7 +2403,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>34</v>
       </c>
@@ -2429,7 +2424,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>35</v>
       </c>
@@ -2450,7 +2445,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>36</v>
       </c>
@@ -2469,7 +2464,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>37</v>
       </c>
@@ -2485,7 +2480,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="27.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>38</v>
       </c>
@@ -2508,7 +2503,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>39</v>
       </c>
@@ -2642,7 +2637,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>46</v>
       </c>
@@ -2663,7 +2658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>47</v>
       </c>
@@ -2696,7 +2691,7 @@
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
     </row>
-    <row r="49" spans="1:7" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>49</v>
       </c>
@@ -2731,7 +2726,7 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
     </row>
-    <row r="51" spans="1:7" ht="26.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>51</v>
       </c>
@@ -2752,7 +2747,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>52</v>
       </c>
@@ -2785,7 +2780,7 @@
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>54</v>
       </c>
@@ -2808,7 +2803,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>55</v>
       </c>
@@ -2829,7 +2824,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>56</v>
       </c>
@@ -2850,7 +2845,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>57</v>
       </c>
@@ -2871,7 +2866,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>58</v>
       </c>
@@ -2910,7 +2905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>60</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>61</v>
       </c>
@@ -2952,7 +2947,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>62</v>
       </c>
@@ -2975,7 +2970,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>63</v>
       </c>
@@ -3014,7 +3009,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>65</v>
       </c>
@@ -3081,8 +3076,8 @@
         <v>48</v>
       </c>
       <c r="E68" s="9"/>
-      <c r="F68" s="9" t="s">
-        <v>134</v>
+      <c r="F68" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3176,6 +3171,7 @@
     <filterColumn colId="5">
       <filters blank="1">
         <filter val="Doing"/>
+        <filter val="Done"/>
         <filter val="New"/>
         <filter val="On Hold"/>
         <filter val="Waiting"/>

</xml_diff>

<commit_message>
hier komt een opmerking, de m staat voor master
</commit_message>
<xml_diff>
--- a/Documentation/Feedback_TBA_Website.xlsx
+++ b/Documentation/Feedback_TBA_Website.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heermti\Desktop\Documents\TBA\Website\TurtoiseDocs\trunk\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="157">
   <si>
     <t>Feedback</t>
   </si>
@@ -493,10 +488,17 @@
     <t>Updaten lay-out referenties</t>
   </si>
   <si>
-    <t>Toevoegen adres Kortrijk</t>
-  </si>
-  <si>
     <t>Cliff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toevoegen adres Kortrijk
+Nelson Mandelaplein 2A 
+BE-8500 Kortrijk 
+België
+</t>
+  </si>
+  <si>
+    <t>release 08/03</t>
   </si>
 </sst>
 </file>
@@ -1765,7 +1767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1777,8 +1779,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I67" sqref="I67"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,13 +3052,16 @@
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E66" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="53" t="s">
-        <v>134</v>
+      <c r="F66" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -3107,22 +3112,27 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>70</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="C70" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D70" s="15"/>
+      <c r="D70" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E70" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F70" s="53" t="s">
-        <v>134</v>
+      <c r="F70" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>